<commit_message>
added new columns to rq22-23 for dre server ph1 adms
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ2.2_2.3_PH1.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ2.2_2.3_PH1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Variables</t>
   </si>
@@ -46,12 +46,24 @@
     <t>Aligned Server Session ID</t>
   </si>
   <si>
+    <t>DRE Aligned ADM Alignment Score (ADM|target)</t>
+  </si>
+  <si>
+    <t>DRE Aligned Server Session ID</t>
+  </si>
+  <si>
     <t>Baseline ADM Alignment score (ADM|target)</t>
   </si>
   <si>
     <t>Baseline Server Session ID</t>
   </si>
   <si>
+    <t>DRE Baseline ADM Alignment score (ADM|target)</t>
+  </si>
+  <si>
+    <t>DRE Baseline Server Session ID</t>
+  </si>
+  <si>
     <t>Source</t>
   </si>
   <si>
@@ -64,6 +76,12 @@
     <t>ADM output/TA1 Server</t>
   </si>
   <si>
+    <t>DRE TA1 Server</t>
+  </si>
+  <si>
+    <t>ADM output/TA1 Server (DRE)</t>
+  </si>
+  <si>
     <t>Definition</t>
   </si>
   <si>
@@ -73,10 +91,16 @@
     <t>The session id used to get the alignment value of the aligned ADM at the specified target from the TA1 server</t>
   </si>
   <si>
+    <t>The session id used to get the alignment value of the aligned ADM at the specified target from the DRE TA1 server</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
     <t>The session id used to get the alignment of the baseline ADM at the specified target from the TA1 server</t>
+  </si>
+  <si>
+    <t>The session id used to get the alignment of the baseline ADM at the specified target from the DRE TA1 server</t>
   </si>
   <si>
     <t>Levels</t>
@@ -150,13 +174,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -469,27 +490,31 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="43.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="69.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="26.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="43.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="69.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="3" width="102.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="3" width="13.005" customWidth="1" bestFit="1" hidden="1"/>
+    <col min="16" max="16" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,47 +551,71 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="211.5">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -576,49 +625,71 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>